<commit_message>
DDLs e DMLs prontos
</commit_message>
<xml_diff>
--- a/Exercicios/1.3-exercicio-pclinics/Fisico.xlsx
+++ b/Exercicios/1.3-exercicio-pclinics/Fisico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Desenvolvimento web senai\2 Semestre\Senai_2S_Sprint1_bd\Exercicios\1.3-exercicio-pclinics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23B1ED13-2BE7-4733-85AF-A218882FF07F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B3A0FE-5C88-4D25-9B0B-0C55EA2D6178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CFF224CB-E1ED-439C-BBE7-700537AA903A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Clinica</t>
   </si>
@@ -111,9 +111,6 @@
     <t xml:space="preserve">                                                              Atendimento                                                     </t>
   </si>
   <si>
-    <t xml:space="preserve">                           Pet          </t>
-  </si>
-  <si>
     <t xml:space="preserve">             Dono</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t xml:space="preserve">                    Tipo       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                      Pet                       </t>
   </si>
 </sst>
 </file>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63492883-B652-4548-A203-5CCFAA22F156}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +515,7 @@
     <col min="18" max="18" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -534,12 +534,13 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="O1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -582,8 +583,11 @@
       <c r="Q2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -626,8 +630,11 @@
       <c r="Q3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
         <v>2</v>
       </c>
@@ -664,8 +671,11 @@
       <c r="Q4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
         <v>3</v>
       </c>
@@ -694,22 +704,22 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -732,7 +742,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -755,7 +765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -778,7 +788,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <v>3</v>
       </c>

</xml_diff>